<commit_message>
latest working code added
</commit_message>
<xml_diff>
--- a/Summary_report_table_count.xlsx
+++ b/Summary_report_table_count.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dixitp\OneDrive - International Shared Support Centre\Dixit_Work\Hawaii_Forest_Trail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://isscindia-my.sharepoint.com/personal/dixitp_issc_co_in/Documents/Dixit_Work/Hawaii_Forest_Trail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2A65B0-A056-4512-895B-9A3E2DC23604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{4B2A65B0-A056-4512-895B-9A3E2DC23604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E35321D-3E0A-43B3-A22B-6B3804B8B79D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Duckdb" sheetId="1" r:id="rId1"/>
     <sheet name="SQL_Server" sheetId="2" r:id="rId2"/>
     <sheet name="Validation" sheetId="3" r:id="rId3"/>
+    <sheet name="TransactionType" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Duckdb!$A$1:$D$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SQL_Server!$A$1:$D$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TransactionType!$A$1:$C$53</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Validation!$A$2:$F$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="70">
   <si>
     <t>database_name</t>
   </si>
@@ -229,6 +231,30 @@
   </si>
   <si>
     <t>Row Count Duckdb</t>
+  </si>
+  <si>
+    <t>Migration Status</t>
+  </si>
+  <si>
+    <t>Migrated</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Type</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>Transaction</t>
+  </si>
+  <si>
+    <t>Line item</t>
   </si>
 </sst>
 </file>
@@ -386,10 +412,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -398,29 +423,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,16 +739,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -731,13 +756,13 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>254</v>
       </c>
     </row>
@@ -745,13 +770,13 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>1055</v>
       </c>
     </row>
@@ -759,13 +784,13 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>6928</v>
       </c>
     </row>
@@ -773,13 +798,13 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>4826</v>
       </c>
     </row>
@@ -787,13 +812,13 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>7278</v>
       </c>
     </row>
@@ -801,13 +826,13 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>9692</v>
       </c>
     </row>
@@ -815,13 +840,13 @@
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>20</v>
       </c>
     </row>
@@ -829,13 +854,13 @@
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>1</v>
       </c>
     </row>
@@ -843,13 +868,13 @@
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>150</v>
       </c>
     </row>
@@ -857,13 +882,13 @@
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>514</v>
       </c>
     </row>
@@ -871,13 +896,13 @@
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>328</v>
       </c>
     </row>
@@ -885,13 +910,13 @@
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>14</v>
       </c>
     </row>
@@ -899,13 +924,13 @@
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>4</v>
       </c>
     </row>
@@ -913,13 +938,13 @@
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>3682</v>
       </c>
     </row>
@@ -927,13 +952,13 @@
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>15124</v>
       </c>
     </row>
@@ -941,13 +966,13 @@
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>1</v>
       </c>
     </row>
@@ -955,13 +980,13 @@
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>21</v>
       </c>
     </row>
@@ -969,13 +994,13 @@
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>43</v>
       </c>
     </row>
@@ -983,13 +1008,13 @@
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>3181</v>
       </c>
     </row>
@@ -997,13 +1022,13 @@
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>8380</v>
       </c>
     </row>
@@ -1011,13 +1036,13 @@
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>866</v>
       </c>
     </row>
@@ -1025,13 +1050,13 @@
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>5039</v>
       </c>
     </row>
@@ -1039,13 +1064,13 @@
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>20186</v>
       </c>
     </row>
@@ -1053,13 +1078,13 @@
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>622</v>
       </c>
     </row>
@@ -1067,13 +1092,13 @@
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <v>2684</v>
       </c>
     </row>
@@ -1081,13 +1106,13 @@
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>15</v>
       </c>
     </row>
@@ -1095,13 +1120,13 @@
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>3946</v>
       </c>
     </row>
@@ -1109,13 +1134,13 @@
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1123,13 +1148,13 @@
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>7287</v>
       </c>
     </row>
@@ -1137,13 +1162,13 @@
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>10016</v>
       </c>
     </row>
@@ -1151,13 +1176,13 @@
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>669</v>
       </c>
     </row>
@@ -1165,13 +1190,13 @@
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>671</v>
       </c>
     </row>
@@ -1179,13 +1204,13 @@
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <v>10604</v>
       </c>
     </row>
@@ -1193,13 +1218,13 @@
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>42206</v>
       </c>
     </row>
@@ -1207,13 +1232,13 @@
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1221,13 +1246,13 @@
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>16</v>
       </c>
     </row>
@@ -1235,13 +1260,13 @@
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>16</v>
       </c>
     </row>
@@ -1249,13 +1274,13 @@
       <c r="A39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>33</v>
       </c>
     </row>
@@ -1263,13 +1288,13 @@
       <c r="A40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1277,13 +1302,13 @@
       <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="3">
         <v>2044</v>
       </c>
     </row>
@@ -1291,13 +1316,13 @@
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>988</v>
       </c>
     </row>
@@ -1305,13 +1330,13 @@
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>80</v>
       </c>
     </row>
@@ -1319,27 +1344,27 @@
       <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="6" t="s">
+      <c r="A45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="6">
         <v>44</v>
       </c>
     </row>
@@ -1366,16 +1391,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1383,13 +1408,13 @@
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>254</v>
       </c>
     </row>
@@ -1397,13 +1422,13 @@
       <c r="A3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>1055</v>
       </c>
     </row>
@@ -1411,13 +1436,13 @@
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>6928</v>
       </c>
     </row>
@@ -1425,13 +1450,13 @@
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>9692</v>
       </c>
     </row>
@@ -1439,13 +1464,13 @@
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>4826</v>
       </c>
     </row>
@@ -1453,13 +1478,13 @@
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>7278</v>
       </c>
     </row>
@@ -1467,13 +1492,13 @@
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>20</v>
       </c>
     </row>
@@ -1481,13 +1506,13 @@
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1495,13 +1520,13 @@
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>150</v>
       </c>
     </row>
@@ -1509,13 +1534,13 @@
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>514</v>
       </c>
     </row>
@@ -1523,13 +1548,13 @@
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>328</v>
       </c>
     </row>
@@ -1537,13 +1562,13 @@
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>14</v>
       </c>
     </row>
@@ -1551,13 +1576,13 @@
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>4</v>
       </c>
     </row>
@@ -1565,13 +1590,13 @@
       <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>3682</v>
       </c>
     </row>
@@ -1579,13 +1604,13 @@
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>15124</v>
       </c>
     </row>
@@ -1593,13 +1618,13 @@
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1607,13 +1632,13 @@
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>21</v>
       </c>
     </row>
@@ -1621,13 +1646,13 @@
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>43</v>
       </c>
     </row>
@@ -1635,13 +1660,13 @@
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>3181</v>
       </c>
     </row>
@@ -1649,13 +1674,13 @@
       <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>8380</v>
       </c>
     </row>
@@ -1663,13 +1688,13 @@
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>866</v>
       </c>
     </row>
@@ -1677,13 +1702,13 @@
       <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>5039</v>
       </c>
     </row>
@@ -1691,13 +1716,13 @@
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>20186</v>
       </c>
     </row>
@@ -1705,13 +1730,13 @@
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>622</v>
       </c>
     </row>
@@ -1719,13 +1744,13 @@
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <v>2684</v>
       </c>
     </row>
@@ -1733,13 +1758,13 @@
       <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>3946</v>
       </c>
     </row>
@@ -1747,13 +1772,13 @@
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>15</v>
       </c>
     </row>
@@ -1761,13 +1786,13 @@
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1775,13 +1800,13 @@
       <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>7287</v>
       </c>
     </row>
@@ -1789,13 +1814,13 @@
       <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>10016</v>
       </c>
     </row>
@@ -1803,13 +1828,13 @@
       <c r="A32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>669</v>
       </c>
     </row>
@@ -1817,13 +1842,13 @@
       <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>671</v>
       </c>
     </row>
@@ -1831,13 +1856,13 @@
       <c r="A34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <v>10604</v>
       </c>
     </row>
@@ -1845,13 +1870,13 @@
       <c r="A35" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>42206</v>
       </c>
     </row>
@@ -1859,13 +1884,13 @@
       <c r="A36" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1873,13 +1898,13 @@
       <c r="A37" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>16</v>
       </c>
     </row>
@@ -1887,13 +1912,13 @@
       <c r="A38" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>16</v>
       </c>
     </row>
@@ -1901,13 +1926,13 @@
       <c r="A39" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>33</v>
       </c>
     </row>
@@ -1915,13 +1940,13 @@
       <c r="A40" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1929,13 +1954,13 @@
       <c r="A41" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="3">
         <v>2044</v>
       </c>
     </row>
@@ -1943,13 +1968,13 @@
       <c r="A42" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>988</v>
       </c>
     </row>
@@ -1957,13 +1982,13 @@
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>80</v>
       </c>
     </row>
@@ -1971,27 +1996,27 @@
       <c r="A44" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="6" t="s">
+      <c r="A45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="6">
         <v>44</v>
       </c>
     </row>
@@ -2005,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FFC03D-7B9F-4034-B7B4-DFA6C31FB766}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2015,1182 +2040,1182 @@
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="str">
+      <c r="A3" s="11" t="str">
         <f>Duckdb!C2</f>
         <v>Account</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <f>VLOOKUP(A3,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>254</v>
       </c>
-      <c r="C3" s="19" t="str">
+      <c r="C3" s="16" t="str">
         <f>SQL_Server!C2</f>
         <v>Account</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="16">
         <f>VLOOKUP(C3,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>254</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="12">
         <f>VLOOKUP(C3,$A$3:$B$46,2,FALSE)</f>
         <v>254</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <f>E3-D3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="str">
+      <c r="A4" s="11" t="str">
         <f>Duckdb!C3</f>
         <v>Attachable</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <f>VLOOKUP(A4,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>1055</v>
       </c>
-      <c r="C4" s="19" t="str">
+      <c r="C4" s="16" t="str">
         <f>SQL_Server!C3</f>
         <v>Attachable</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="16">
         <f>VLOOKUP(C4,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>1055</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="12">
         <f t="shared" ref="E4:E46" si="0">VLOOKUP(C4,$A$3:$B$46,2,FALSE)</f>
         <v>1055</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f t="shared" ref="F4:F46" si="1">E4-D4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="str">
+      <c r="A5" s="11" t="str">
         <f>Duckdb!C4</f>
         <v>Bill</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <f>VLOOKUP(A5,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>6928</v>
       </c>
-      <c r="C5" s="19" t="str">
+      <c r="C5" s="16" t="str">
         <f>SQL_Server!C4</f>
         <v>Bill</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="16">
         <f>VLOOKUP(C5,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>6928</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="12">
         <f t="shared" si="0"/>
         <v>6928</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="str">
+      <c r="A6" s="11" t="str">
         <f>Duckdb!C5</f>
         <v>BillPayment</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <f>VLOOKUP(A6,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>4826</v>
       </c>
-      <c r="C6" s="19" t="str">
+      <c r="C6" s="16" t="str">
         <f>SQL_Server!C5</f>
         <v>Bill_Line</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="16">
         <f>VLOOKUP(C6,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>9692</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <f t="shared" si="0"/>
         <v>9692</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="str">
+      <c r="A7" s="11" t="str">
         <f>Duckdb!C6</f>
         <v>BillPayment_Line</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <f>VLOOKUP(A7,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>7278</v>
       </c>
-      <c r="C7" s="19" t="str">
+      <c r="C7" s="16" t="str">
         <f>SQL_Server!C6</f>
         <v>BillPayment</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="16">
         <f>VLOOKUP(C7,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>4826</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="12">
         <f t="shared" si="0"/>
         <v>4826</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="str">
+      <c r="A8" s="11" t="str">
         <f>Duckdb!C7</f>
         <v>Bill_Line</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <f>VLOOKUP(A8,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>9692</v>
       </c>
-      <c r="C8" s="19" t="str">
+      <c r="C8" s="16" t="str">
         <f>SQL_Server!C7</f>
         <v>BillPayment_Line</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="16">
         <f>VLOOKUP(C8,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>7278</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <f t="shared" si="0"/>
         <v>7278</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="str">
+      <c r="A9" s="11" t="str">
         <f>Duckdb!C8</f>
         <v>Class</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="12">
         <f>VLOOKUP(A9,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>20</v>
       </c>
-      <c r="C9" s="19" t="str">
+      <c r="C9" s="16" t="str">
         <f>SQL_Server!C8</f>
         <v>Class</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="16">
         <f>VLOOKUP(C9,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>20</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="12">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="str">
+      <c r="A10" s="11" t="str">
         <f>Duckdb!C9</f>
         <v>CompanyInfo</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <f>VLOOKUP(A10,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="C10" s="19" t="str">
+      <c r="C10" s="16" t="str">
         <f>SQL_Server!C9</f>
         <v>CompanyInfo</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="16">
         <f>VLOOKUP(C10,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="str">
+      <c r="A11" s="11" t="str">
         <f>Duckdb!C10</f>
         <v>CreditMemo</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="12">
         <f>VLOOKUP(A11,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>150</v>
       </c>
-      <c r="C11" s="19" t="str">
+      <c r="C11" s="16" t="str">
         <f>SQL_Server!C10</f>
         <v>CreditMemo</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="16">
         <f>VLOOKUP(C11,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>150</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="str">
+      <c r="A12" s="11" t="str">
         <f>Duckdb!C11</f>
         <v>CreditMemo_Line</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="12">
         <f>VLOOKUP(A12,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>514</v>
       </c>
-      <c r="C12" s="19" t="str">
+      <c r="C12" s="16" t="str">
         <f>SQL_Server!C11</f>
         <v>CreditMemo_Line</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="16">
         <f>VLOOKUP(C12,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>514</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="12">
         <f t="shared" si="0"/>
         <v>514</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="str">
+      <c r="A13" s="11" t="str">
         <f>Duckdb!C12</f>
         <v>Customer</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="12">
         <f>VLOOKUP(A13,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>328</v>
       </c>
-      <c r="C13" s="19" t="str">
+      <c r="C13" s="16" t="str">
         <f>SQL_Server!C12</f>
         <v>Customer</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="16">
         <f>VLOOKUP(C13,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>328</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="12">
         <f t="shared" si="0"/>
         <v>328</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="str">
+      <c r="A14" s="11" t="str">
         <f>Duckdb!C13</f>
         <v>CustomerType</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="12">
         <f>VLOOKUP(A14,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>14</v>
       </c>
-      <c r="C14" s="19" t="str">
+      <c r="C14" s="16" t="str">
         <f>SQL_Server!C13</f>
         <v>CustomerType</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="16">
         <f>VLOOKUP(C14,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>14</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="12">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="str">
+      <c r="A15" s="11" t="str">
         <f>Duckdb!C14</f>
         <v>Department</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="12">
         <f>VLOOKUP(A15,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="C15" s="19" t="str">
+      <c r="C15" s="16" t="str">
         <f>SQL_Server!C14</f>
         <v>Department</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="16">
         <f>VLOOKUP(C15,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="E15" s="15">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="E15" s="12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F15" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="str">
+      <c r="A16" s="11" t="str">
         <f>Duckdb!C15</f>
         <v>Deposit</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="12">
         <f>VLOOKUP(A16,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>3682</v>
       </c>
-      <c r="C16" s="19" t="str">
+      <c r="C16" s="16" t="str">
         <f>SQL_Server!C15</f>
         <v>Deposit</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="16">
         <f>VLOOKUP(C16,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>3682</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="12">
         <f t="shared" si="0"/>
         <v>3682</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="str">
+      <c r="A17" s="11" t="str">
         <f>Duckdb!C16</f>
         <v>Deposit_Line</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="12">
         <f>VLOOKUP(A17,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>15124</v>
       </c>
-      <c r="C17" s="19" t="str">
+      <c r="C17" s="16" t="str">
         <f>SQL_Server!C16</f>
         <v>Deposit_Line</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="16">
         <f>VLOOKUP(C17,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>15124</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="12">
         <f t="shared" si="0"/>
         <v>15124</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="str">
+      <c r="A18" s="11" t="str">
         <f>Duckdb!C17</f>
         <v>Employee</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="12">
         <f>VLOOKUP(A18,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="C18" s="19" t="str">
+      <c r="C18" s="16" t="str">
         <f>SQL_Server!C17</f>
         <v>Employee</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="16">
         <f>VLOOKUP(C18,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="str">
+      <c r="A19" s="11" t="str">
         <f>Duckdb!C18</f>
         <v>Estimate</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="12">
         <f>VLOOKUP(A19,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>21</v>
       </c>
-      <c r="C19" s="19" t="str">
+      <c r="C19" s="16" t="str">
         <f>SQL_Server!C18</f>
         <v>Estimate</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="16">
         <f>VLOOKUP(C19,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>21</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="12">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="str">
+      <c r="A20" s="11" t="str">
         <f>Duckdb!C19</f>
         <v>Estimate_Line</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="12">
         <f>VLOOKUP(A20,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>43</v>
       </c>
-      <c r="C20" s="19" t="str">
+      <c r="C20" s="16" t="str">
         <f>SQL_Server!C19</f>
         <v>Estimate_Line</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="16">
         <f>VLOOKUP(C20,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>43</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="12">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="str">
+      <c r="A21" s="11" t="str">
         <f>Duckdb!C20</f>
         <v>Invoice</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="12">
         <f>VLOOKUP(A21,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>3181</v>
       </c>
-      <c r="C21" s="19" t="str">
+      <c r="C21" s="16" t="str">
         <f>SQL_Server!C20</f>
         <v>Invoice</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="16">
         <f>VLOOKUP(C21,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>3181</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="12">
         <f t="shared" si="0"/>
         <v>3181</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="str">
+      <c r="A22" s="11" t="str">
         <f>Duckdb!C21</f>
         <v>Invoice_Line</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="12">
         <f>VLOOKUP(A22,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>8380</v>
       </c>
-      <c r="C22" s="19" t="str">
+      <c r="C22" s="16" t="str">
         <f>SQL_Server!C21</f>
         <v>Invoice_Line</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="16">
         <f>VLOOKUP(C22,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>8380</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="12">
         <f t="shared" si="0"/>
         <v>8380</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="str">
+      <c r="A23" s="11" t="str">
         <f>Duckdb!C22</f>
         <v>Item</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="12">
         <f>VLOOKUP(A23,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>866</v>
       </c>
-      <c r="C23" s="19" t="str">
+      <c r="C23" s="16" t="str">
         <f>SQL_Server!C22</f>
         <v>Item</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="16">
         <f>VLOOKUP(C23,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>866</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="12">
         <f t="shared" si="0"/>
         <v>866</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="str">
+      <c r="A24" s="11" t="str">
         <f>Duckdb!C23</f>
         <v>JournalEntry</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="12">
         <f>VLOOKUP(A24,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>5039</v>
       </c>
-      <c r="C24" s="19" t="str">
+      <c r="C24" s="16" t="str">
         <f>SQL_Server!C23</f>
         <v>JournalEntry</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="16">
         <f>VLOOKUP(C24,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>5039</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="12">
         <f t="shared" si="0"/>
         <v>5039</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="str">
+      <c r="A25" s="11" t="str">
         <f>Duckdb!C24</f>
         <v>JournalEntry_Line</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="12">
         <f>VLOOKUP(A25,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>20186</v>
       </c>
-      <c r="C25" s="19" t="str">
+      <c r="C25" s="16" t="str">
         <f>SQL_Server!C24</f>
         <v>JournalEntry_Line</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="16">
         <f>VLOOKUP(C25,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>20186</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="12">
         <f t="shared" si="0"/>
         <v>20186</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="str">
+      <c r="A26" s="11" t="str">
         <f>Duckdb!C25</f>
         <v>LinkedTxn</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="12">
         <f>VLOOKUP(A26,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>622</v>
       </c>
-      <c r="C26" s="19" t="str">
+      <c r="C26" s="16" t="str">
         <f>SQL_Server!C25</f>
         <v>LinkedTxn</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="16">
         <f>VLOOKUP(C26,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>622</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="12">
         <f t="shared" si="0"/>
         <v>622</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="str">
+      <c r="A27" s="11" t="str">
         <f>Duckdb!C26</f>
         <v>Payment</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="12">
         <f>VLOOKUP(A27,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>2684</v>
       </c>
-      <c r="C27" s="19" t="str">
+      <c r="C27" s="16" t="str">
         <f>SQL_Server!C26</f>
         <v>Payment</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="16">
         <f>VLOOKUP(C27,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>2684</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="12">
         <f t="shared" si="0"/>
         <v>2684</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="str">
+      <c r="A28" s="11" t="str">
         <f>Duckdb!C27</f>
         <v>PaymentMethod</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="12">
         <f>VLOOKUP(A28,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>15</v>
       </c>
-      <c r="C28" s="19" t="str">
+      <c r="C28" s="16" t="str">
         <f>SQL_Server!C27</f>
         <v>Payment_Line</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="16">
         <f>VLOOKUP(C28,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>3946</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="12">
         <f t="shared" si="0"/>
         <v>3946</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="str">
+      <c r="A29" s="11" t="str">
         <f>Duckdb!C28</f>
         <v>Payment_Line</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="12">
         <f>VLOOKUP(A29,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>3946</v>
       </c>
-      <c r="C29" s="19" t="str">
+      <c r="C29" s="16" t="str">
         <f>SQL_Server!C28</f>
         <v>PaymentMethod</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="16">
         <f>VLOOKUP(C29,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>15</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="12">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="str">
+      <c r="A30" s="11" t="str">
         <f>Duckdb!C29</f>
         <v>Preferences</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="12">
         <f>VLOOKUP(A30,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="C30" s="19" t="str">
+      <c r="C30" s="16" t="str">
         <f>SQL_Server!C29</f>
         <v>Preferences</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="16">
         <f>VLOOKUP(C30,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="str">
+      <c r="A31" s="11" t="str">
         <f>Duckdb!C30</f>
         <v>Purchase</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="12">
         <f>VLOOKUP(A31,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>7287</v>
       </c>
-      <c r="C31" s="19" t="str">
+      <c r="C31" s="16" t="str">
         <f>SQL_Server!C30</f>
         <v>Purchase</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="16">
         <f>VLOOKUP(C31,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>7287</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="12">
         <f t="shared" si="0"/>
         <v>7287</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="str">
+      <c r="A32" s="11" t="str">
         <f>Duckdb!C31</f>
         <v>Purchase_Line</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="12">
         <f>VLOOKUP(A32,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>10016</v>
       </c>
-      <c r="C32" s="19" t="str">
+      <c r="C32" s="16" t="str">
         <f>SQL_Server!C31</f>
         <v>Purchase_Line</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="16">
         <f>VLOOKUP(C32,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>10016</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="12">
         <f t="shared" si="0"/>
         <v>10016</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="str">
+      <c r="A33" s="11" t="str">
         <f>Duckdb!C32</f>
         <v>ReimburseCharge</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="12">
         <f>VLOOKUP(A33,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>669</v>
       </c>
-      <c r="C33" s="19" t="str">
+      <c r="C33" s="16" t="str">
         <f>SQL_Server!C32</f>
         <v>ReimburseCharge</v>
       </c>
-      <c r="D33" s="19">
+      <c r="D33" s="16">
         <f>VLOOKUP(C33,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>669</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="12">
         <f t="shared" si="0"/>
         <v>669</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="str">
+      <c r="A34" s="11" t="str">
         <f>Duckdb!C33</f>
         <v>ReimburseCharge_Line</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="12">
         <f>VLOOKUP(A34,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>671</v>
       </c>
-      <c r="C34" s="19" t="str">
+      <c r="C34" s="16" t="str">
         <f>SQL_Server!C33</f>
         <v>ReimburseCharge_Line</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D34" s="16">
         <f>VLOOKUP(C34,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>671</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="12">
         <f t="shared" si="0"/>
         <v>671</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="str">
+      <c r="A35" s="11" t="str">
         <f>Duckdb!C34</f>
         <v>SalesReceipt</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="12">
         <f>VLOOKUP(A35,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>10604</v>
       </c>
-      <c r="C35" s="19" t="str">
+      <c r="C35" s="16" t="str">
         <f>SQL_Server!C34</f>
         <v>SalesReceipt</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="16">
         <f>VLOOKUP(C35,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>10604</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="12">
         <f t="shared" si="0"/>
         <v>10604</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="str">
+      <c r="A36" s="11" t="str">
         <f>Duckdb!C35</f>
         <v>SalesReceipt_Line</v>
       </c>
-      <c r="B36" s="15">
+      <c r="B36" s="12">
         <f>VLOOKUP(A36,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>42206</v>
       </c>
-      <c r="C36" s="19" t="str">
+      <c r="C36" s="16" t="str">
         <f>SQL_Server!C35</f>
         <v>SalesReceipt_Line</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D36" s="16">
         <f>VLOOKUP(C36,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>42206</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="12">
         <f t="shared" si="0"/>
         <v>42206</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="str">
+      <c r="A37" s="11" t="str">
         <f>Duckdb!C36</f>
         <v>TaxAgency</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="12">
         <f>VLOOKUP(A37,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="C37" s="19" t="str">
+      <c r="C37" s="16" t="str">
         <f>SQL_Server!C36</f>
         <v>TaxAgency</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D37" s="16">
         <f>VLOOKUP(C37,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="12">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="str">
+      <c r="A38" s="11" t="str">
         <f>Duckdb!C37</f>
         <v>TaxCode</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="12">
         <f>VLOOKUP(A38,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>16</v>
       </c>
-      <c r="C38" s="19" t="str">
+      <c r="C38" s="16" t="str">
         <f>SQL_Server!C37</f>
         <v>TaxCode</v>
       </c>
-      <c r="D38" s="19">
+      <c r="D38" s="16">
         <f>VLOOKUP(C38,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>16</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="12">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="str">
+      <c r="A39" s="11" t="str">
         <f>Duckdb!C38</f>
         <v>TaxRate</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="12">
         <f>VLOOKUP(A39,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>16</v>
       </c>
-      <c r="C39" s="19" t="str">
+      <c r="C39" s="16" t="str">
         <f>SQL_Server!C38</f>
         <v>TaxRate</v>
       </c>
-      <c r="D39" s="19">
+      <c r="D39" s="16">
         <f>VLOOKUP(C39,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>16</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="12">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="str">
+      <c r="A40" s="11" t="str">
         <f>Duckdb!C39</f>
         <v>Term</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="12">
         <f>VLOOKUP(A40,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>33</v>
       </c>
-      <c r="C40" s="19" t="str">
+      <c r="C40" s="16" t="str">
         <f>SQL_Server!C39</f>
         <v>Term</v>
       </c>
-      <c r="D40" s="19">
+      <c r="D40" s="16">
         <f>VLOOKUP(C40,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>33</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="12">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="str">
+      <c r="A41" s="11" t="str">
         <f>Duckdb!C40</f>
         <v>TimeActivity</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B41" s="12">
         <f>VLOOKUP(A41,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="C41" s="19" t="str">
+      <c r="C41" s="16" t="str">
         <f>SQL_Server!C40</f>
         <v>TimeActivity</v>
       </c>
-      <c r="D41" s="19">
+      <c r="D41" s="16">
         <f>VLOOKUP(C41,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="12">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="str">
+      <c r="A42" s="11" t="str">
         <f>Duckdb!C41</f>
         <v>Transfer</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B42" s="12">
         <f>VLOOKUP(A42,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>2044</v>
       </c>
-      <c r="C42" s="19" t="str">
+      <c r="C42" s="16" t="str">
         <f>SQL_Server!C41</f>
         <v>Transfer</v>
       </c>
-      <c r="D42" s="19">
+      <c r="D42" s="16">
         <f>VLOOKUP(C42,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>2044</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="12">
         <f t="shared" si="0"/>
         <v>2044</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="str">
+      <c r="A43" s="11" t="str">
         <f>Duckdb!C42</f>
         <v>Vendor</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="12">
         <f>VLOOKUP(A43,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>988</v>
       </c>
-      <c r="C43" s="19" t="str">
+      <c r="C43" s="16" t="str">
         <f>SQL_Server!C42</f>
         <v>Vendor</v>
       </c>
-      <c r="D43" s="19">
+      <c r="D43" s="16">
         <f>VLOOKUP(C43,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>988</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="12">
         <f t="shared" si="0"/>
         <v>988</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="str">
+      <c r="A44" s="11" t="str">
         <f>Duckdb!C43</f>
         <v>VendorCredit</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="12">
         <f>VLOOKUP(A44,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>80</v>
       </c>
-      <c r="C44" s="19" t="str">
+      <c r="C44" s="16" t="str">
         <f>SQL_Server!C43</f>
         <v>VendorCredit</v>
       </c>
-      <c r="D44" s="19">
+      <c r="D44" s="16">
         <f>VLOOKUP(C44,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>80</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="12">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="str">
+      <c r="A45" s="11" t="str">
         <f>Duckdb!C44</f>
         <v>VendorCredit_Line</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="12">
         <f>VLOOKUP(A45,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>105</v>
       </c>
-      <c r="C45" s="19" t="str">
+      <c r="C45" s="16" t="str">
         <f>SQL_Server!C44</f>
         <v>VendorCredit_Line</v>
       </c>
-      <c r="D45" s="19">
+      <c r="D45" s="16">
         <f>VLOOKUP(C45,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>105</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="12">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="str">
+      <c r="A46" s="13" t="str">
         <f>Duckdb!C45</f>
         <v>Extraction_Status</v>
       </c>
-      <c r="B46" s="17">
+      <c r="B46" s="14">
         <f>VLOOKUP(A46,Duckdb!$C$2:$D$45,2,FALSE)</f>
         <v>44</v>
       </c>
-      <c r="C46" s="20" t="str">
+      <c r="C46" s="17" t="str">
         <f>SQL_Server!C45</f>
         <v>Extraction_Status</v>
       </c>
-      <c r="D46" s="20">
+      <c r="D46" s="17">
         <f>VLOOKUP(C46,SQL_Server!$C$2:$D$45,2,FALSE)</f>
         <v>44</v>
       </c>
-      <c r="E46" s="17">
+      <c r="E46" s="14">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F46" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3203,4 +3228,601 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99B9677-4A0F-4BB0-9523-4AF2E9961E8F}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:C53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <f>Validation!A3</f>
+        <v>Account</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="str">
+        <f>Validation!A4</f>
+        <v>Attachable</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="str">
+        <f>Validation!A5</f>
+        <v>Bill</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="str">
+        <f>Validation!A6</f>
+        <v>BillPayment</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="str">
+        <f>Validation!A7</f>
+        <v>BillPayment_Line</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="str">
+        <f>Validation!A8</f>
+        <v>Bill_Line</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="str">
+        <f>Validation!A9</f>
+        <v>Class</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <f>Validation!A10</f>
+        <v>CompanyInfo</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <f>Validation!A11</f>
+        <v>CreditMemo</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <f>Validation!A12</f>
+        <v>CreditMemo_Line</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <f>Validation!A13</f>
+        <v>Customer</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <f>Validation!A14</f>
+        <v>CustomerType</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <f>Validation!A15</f>
+        <v>Department</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f>Validation!A16</f>
+        <v>Deposit</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f>Validation!A17</f>
+        <v>Deposit_Line</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f>Validation!A18</f>
+        <v>Employee</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="str">
+        <f>Validation!A19</f>
+        <v>Estimate</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="str">
+        <f>Validation!A20</f>
+        <v>Estimate_Line</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="str">
+        <f>Validation!A21</f>
+        <v>Invoice</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="str">
+        <f>Validation!A22</f>
+        <v>Invoice_Line</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="str">
+        <f>Validation!A23</f>
+        <v>Item</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="str">
+        <f>Validation!A24</f>
+        <v>JournalEntry</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="str">
+        <f>Validation!A25</f>
+        <v>JournalEntry_Line</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="str">
+        <f>Validation!A26</f>
+        <v>LinkedTxn</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="str">
+        <f>Validation!A27</f>
+        <v>Payment</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="str">
+        <f>Validation!A28</f>
+        <v>PaymentMethod</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="str">
+        <f>Validation!A29</f>
+        <v>Payment_Line</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="str">
+        <f>Validation!A30</f>
+        <v>Preferences</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="str">
+        <f>Validation!A31</f>
+        <v>Purchase</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="str">
+        <f>Validation!A32</f>
+        <v>Purchase_Line</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="str">
+        <f>Validation!A33</f>
+        <v>ReimburseCharge</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="str">
+        <f>Validation!A34</f>
+        <v>ReimburseCharge_Line</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="str">
+        <f>Validation!A35</f>
+        <v>SalesReceipt</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="str">
+        <f>Validation!A36</f>
+        <v>SalesReceipt_Line</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="str">
+        <f>Validation!A37</f>
+        <v>TaxAgency</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="str">
+        <f>Validation!A38</f>
+        <v>TaxCode</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="str">
+        <f>Validation!A39</f>
+        <v>TaxRate</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="str">
+        <f>Validation!A40</f>
+        <v>Term</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="str">
+        <f>Validation!A41</f>
+        <v>TimeActivity</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="str">
+        <f>Validation!A42</f>
+        <v>Transfer</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="str">
+        <f>Validation!A43</f>
+        <v>Vendor</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="str">
+        <f>Validation!A44</f>
+        <v>VendorCredit</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="str">
+        <f>Validation!A45</f>
+        <v>VendorCredit_Line</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="24"/>
+    </row>
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="24"/>
+    </row>
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="24"/>
+    </row>
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="24"/>
+    </row>
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="24"/>
+    </row>
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="24"/>
+    </row>
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="24"/>
+    </row>
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="24"/>
+    </row>
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="24"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C53" xr:uid="{B99B9677-4A0F-4BB0-9523-4AF2E9961E8F}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Transaction"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{42259CEC-87F0-49E9-9F0E-CB491CC9BDB3}">
+      <formula1>"Migrated, NA, Pending"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>